<commit_message>
Commit for changes and new script for fee reports
</commit_message>
<xml_diff>
--- a/src/main/java/com/test/automation/uiAutomation/data/FeeReportsData.xlsx
+++ b/src/main/java/com/test/automation/uiAutomation/data/FeeReportsData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8370" firstSheet="9" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8370" firstSheet="14" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="DailyCollectionReport" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,17 @@
     <sheet name="Search_YearlyFeeConcession" sheetId="10" r:id="rId10"/>
     <sheet name="FeeDueDates_Report" sheetId="11" r:id="rId11"/>
     <sheet name="Search_FeeDueDatesReport" sheetId="12" r:id="rId12"/>
+    <sheet name="FeeMonthEnd_Report" sheetId="13" r:id="rId13"/>
+    <sheet name="FeeITReceipt_Report" sheetId="14" r:id="rId14"/>
+    <sheet name="Fee_MonthlyCollectionData_AdmNo" sheetId="15" r:id="rId15"/>
+    <sheet name="Fee_MonthlyCollectionData_Name" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="30">
   <si>
     <t>Academic Year</t>
   </si>
@@ -100,13 +104,28 @@
   </si>
   <si>
     <t>Computer Fees</t>
+  </si>
+  <si>
+    <t>Receipt Number</t>
+  </si>
+  <si>
+    <t>18106</t>
+  </si>
+  <si>
+    <t>Some One</t>
+  </si>
+  <si>
+    <t>1233546-Dinesh Tamada</t>
+  </si>
+  <si>
+    <t>Dinesh Tamada-1233546</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +176,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -178,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -213,6 +245,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,7 +637,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -644,7 +678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -674,6 +708,170 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>

</xml_diff>

<commit_message>
Commit for Fee Installment Report
</commit_message>
<xml_diff>
--- a/src/main/java/com/test/automation/uiAutomation/data/FeeReportsData.xlsx
+++ b/src/main/java/com/test/automation/uiAutomation/data/FeeReportsData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8370" firstSheet="14" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8370" firstSheet="16" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="DailyCollectionReport" sheetId="1" r:id="rId1"/>
@@ -23,13 +23,15 @@
     <sheet name="FeeITReceipt_Report" sheetId="14" r:id="rId14"/>
     <sheet name="Fee_MonthlyCollectionData_AdmNo" sheetId="15" r:id="rId15"/>
     <sheet name="Fee_MonthlyCollectionData_Name" sheetId="16" r:id="rId16"/>
+    <sheet name="FeeInstallment_CategoryWise" sheetId="17" r:id="rId17"/>
+    <sheet name="FeeInstallment_ClassWise" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="32">
   <si>
     <t>Academic Year</t>
   </si>
@@ -119,18 +121,31 @@
   </si>
   <si>
     <t>Dinesh Tamada-1233546</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Seaction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -210,12 +225,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -227,26 +242,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,7 +863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -872,6 +893,94 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>

</xml_diff>